<commit_message>
Updated USA model - 2025-07-29 08:49
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/vt_vervestacks_USA_v1.xlsx
+++ b/VerveStacks_USA/vt_vervestacks_USA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84A19BD9-A2C2-435F-A670-684C98231530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68EECFFD-AF7F-4652-AEF3-FC23B7D5915E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{97829B8E-8E95-4E17-B067-ABAE40F0E90C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{CE40F399-E00A-4E3E-AD69-23535139E940}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -6684,7 +6684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779CC8FB-2F17-429E-8908-0B0B8C8B2C97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9036EB-C672-4007-ABDD-1DC0AD30ECC6}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -9609,7 +9609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9707A5F-6447-459F-BB09-D473DDAC4753}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB33BD31-CE2C-47ED-A234-69B3B13942F8}">
   <dimension ref="A2:T440"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -34158,7 +34158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7B05A7-4134-48CF-A67D-B90A79DA3BEB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE0BE79-C5E6-4022-B681-CA4B2C4A8202}">
   <dimension ref="A2:S1211"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated USA model - 2025-07-29 09:00
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/vt_vervestacks_USA_v1.xlsx
+++ b/VerveStacks_USA/vt_vervestacks_USA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68EECFFD-AF7F-4652-AEF3-FC23B7D5915E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20D2C172-F099-496E-9D76-A0241002E509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{CE40F399-E00A-4E3E-AD69-23535139E940}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{36C0E80B-C44E-4076-93C3-48931DAA267F}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -6684,7 +6684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9036EB-C672-4007-ABDD-1DC0AD30ECC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5F373D-6F8B-4F6D-8B4A-E0C8192C56C1}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -9609,7 +9609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB33BD31-CE2C-47ED-A234-69B3B13942F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E03380-903B-4416-B6FF-0734FA2C64B7}">
   <dimension ref="A2:T440"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -34158,7 +34158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE0BE79-C5E6-4022-B681-CA4B2C4A8202}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8417D19E-C923-4206-87C2-DC58DD3767DE}">
   <dimension ref="A2:S1211"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated USA model - 2025-07-29 09:11
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/vt_vervestacks_USA_v1.xlsx
+++ b/VerveStacks_USA/vt_vervestacks_USA_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20D2C172-F099-496E-9D76-A0241002E509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AFF946D-94C9-412E-90A5-D1B110EAA1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{36C0E80B-C44E-4076-93C3-48931DAA267F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{D87B372C-0374-4809-9B55-E3EA1D71B4DD}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -6684,7 +6684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5F373D-6F8B-4F6D-8B4A-E0C8192C56C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF66F80-2741-46C5-920B-1D9940952F4A}">
   <dimension ref="A2:P107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -9609,7 +9609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E03380-903B-4416-B6FF-0734FA2C64B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D9BC3A-0175-4BCE-8EB6-ED32B6D8C33E}">
   <dimension ref="A2:T440"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -34158,7 +34158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8417D19E-C923-4206-87C2-DC58DD3767DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE73CC5-A479-40FD-9A48-0D27FC8A4837}">
   <dimension ref="A2:S1211"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>